<commit_message>
feat: update weekly report 4/29
</commit_message>
<xml_diff>
--- a/weeklyReport/张鸿斌/张鸿斌-周工作总结excel（工作周报）.xlsx
+++ b/weeklyReport/张鸿斌/张鸿斌-周工作总结excel（工作周报）.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\VSCodeWorkspace\IDPhotoProductionPlatform\weeklyReport\张鸿斌\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6992D0-DC18-4D45-B71A-31C2B474052B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D48E731-C872-45A5-B600-4E4DB1049B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="第五周工作周报" sheetId="7" r:id="rId1"/>
-    <sheet name="第六周工作周报" sheetId="9" r:id="rId2"/>
+    <sheet name="第六周工作周报 " sheetId="11" r:id="rId2"/>
+    <sheet name="第七周工作周报" sheetId="9" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">第六周工作周报!$A$1:$O$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'第六周工作周报 '!$A$1:$O$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">第七周工作周报!$A$1:$O$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">第五周工作周报!$A$1:$O$35</definedName>
   </definedNames>
   <calcPr calcId="114210"/>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="65">
   <si>
     <t>本周工作总结</t>
   </si>
@@ -289,6 +292,33 @@
         <charset val="134"/>
       </rPr>
       <t>：本周主要完成了用户管理模块的开发任务，并撰写整理完成详细设计文档</t>
+    </r>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功修改之前的权限问题BUG</t>
+    <phoneticPr fontId="38" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习使用vuex进行状态管理</t>
+    <phoneticPr fontId="38" type="noConversion"/>
+  </si>
+  <si>
+    <t>已初步完成平台的基本功能</t>
+    <phoneticPr fontId="38" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>本周工作总结</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="幼圆"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>：本周主要完善了平台的基础功能，能够响应基本的用户需求</t>
     </r>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -1191,6 +1221,138 @@
     <xf numFmtId="176" fontId="33" fillId="24" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="58" fontId="33" fillId="24" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="18" xfId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="23" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="24" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="22" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="18" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="21" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="11" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="13" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="13" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="14" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="24" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="24" borderId="11" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="11" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="33" fillId="26" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="24" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1206,140 +1368,14 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="33" fillId="26" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="33" fillId="26" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="11" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="11" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="13" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="13" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="14" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="24" borderId="10" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="24" borderId="11" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="19" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="22" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="18" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="21" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="16" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="23" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="24" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="18" xfId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="19" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="26" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1358,12 +1394,6 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="18" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="33" fillId="26" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="33" fillId="24" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1821,69 +1851,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="49"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="35"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="52"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="38"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
     <row r="3" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="53" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="55"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="41"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
@@ -1892,520 +1922,520 @@
       <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="57"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="43"/>
       <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>1</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
       <c r="G5" s="8">
         <v>1</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="44"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="46"/>
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
       <c r="G6" s="9">
         <v>2</v>
       </c>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="47"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="49"/>
       <c r="P6" s="7"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>3</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
       <c r="G7" s="8">
         <v>3</v>
       </c>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="44"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="46"/>
       <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="37" t="s">
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="40"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="52"/>
       <c r="P8" s="7"/>
     </row>
     <row r="9" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="63" t="s">
+      <c r="E9" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="64"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38" t="s">
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38" t="s">
+      <c r="M9" s="53"/>
+      <c r="N9" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="41"/>
+      <c r="O9" s="54"/>
       <c r="P9" s="7"/>
     </row>
     <row r="10" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="31">
+      <c r="B10" s="63"/>
+      <c r="C10" s="64">
         <v>44662</v>
       </c>
-      <c r="D10" s="65" t="s">
+      <c r="D10" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="67">
+      <c r="E10" s="23">
         <v>0.9</v>
       </c>
-      <c r="F10" s="68"/>
-      <c r="G10" s="32">
+      <c r="F10" s="24"/>
+      <c r="G10" s="61">
         <v>1</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="28"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="62"/>
       <c r="P10" s="7"/>
     </row>
     <row r="11" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="28"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="62"/>
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="31">
+      <c r="B12" s="63"/>
+      <c r="C12" s="64">
         <v>44663</v>
       </c>
-      <c r="D12" s="65" t="s">
+      <c r="D12" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="67">
+      <c r="E12" s="23">
         <v>1</v>
       </c>
-      <c r="F12" s="68"/>
-      <c r="G12" s="32">
+      <c r="F12" s="24"/>
+      <c r="G12" s="61">
         <v>2</v>
       </c>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="28"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="62"/>
       <c r="P12" s="7"/>
     </row>
     <row r="13" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="28"/>
+      <c r="A13" s="63"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="62"/>
       <c r="P13" s="7"/>
     </row>
     <row r="14" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="31">
+      <c r="B14" s="63"/>
+      <c r="C14" s="64">
         <v>44664</v>
       </c>
-      <c r="D14" s="65" t="s">
+      <c r="D14" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="67">
+      <c r="E14" s="23">
         <v>0.1</v>
       </c>
-      <c r="F14" s="68"/>
-      <c r="G14" s="32">
+      <c r="F14" s="24"/>
+      <c r="G14" s="61">
         <v>3</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="28"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="62"/>
       <c r="P14" s="7"/>
     </row>
     <row r="15" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="28"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="62"/>
       <c r="P15" s="7"/>
     </row>
     <row r="16" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="31">
+      <c r="B16" s="63"/>
+      <c r="C16" s="64">
         <v>44665</v>
       </c>
-      <c r="D16" s="65" t="s">
+      <c r="D16" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="67">
+      <c r="E16" s="23">
         <v>0.3</v>
       </c>
-      <c r="F16" s="68"/>
-      <c r="G16" s="32">
+      <c r="F16" s="24"/>
+      <c r="G16" s="61">
         <v>4</v>
       </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="28"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="62"/>
       <c r="P16" s="7"/>
     </row>
     <row r="17" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="28"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="62"/>
       <c r="P17" s="7"/>
     </row>
     <row r="18" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="31">
+      <c r="B18" s="63"/>
+      <c r="C18" s="64">
         <v>44666</v>
       </c>
-      <c r="D18" s="65" t="s">
+      <c r="D18" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="67">
+      <c r="E18" s="23">
         <v>0.5</v>
       </c>
-      <c r="F18" s="68"/>
-      <c r="G18" s="32">
+      <c r="F18" s="24"/>
+      <c r="G18" s="61">
         <v>5</v>
       </c>
-      <c r="H18" s="27"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="58"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="29"/>
       <c r="P18" s="7"/>
     </row>
     <row r="19" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="60"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="31"/>
       <c r="P19" s="7"/>
     </row>
     <row r="20" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="31">
+      <c r="B20" s="63"/>
+      <c r="C20" s="64">
         <v>44667</v>
       </c>
-      <c r="D20" s="65" t="s">
+      <c r="D20" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="67">
+      <c r="E20" s="23">
         <v>0.5</v>
       </c>
-      <c r="F20" s="68"/>
-      <c r="G20" s="32">
+      <c r="F20" s="24"/>
+      <c r="G20" s="61">
         <v>6</v>
       </c>
-      <c r="H20" s="27" t="s">
+      <c r="H20" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="27" t="s">
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="M20" s="58"/>
-      <c r="N20" s="27" t="s">
+      <c r="M20" s="29"/>
+      <c r="N20" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="O20" s="58"/>
+      <c r="O20" s="29"/>
       <c r="P20" s="7"/>
     </row>
     <row r="21" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="60"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="31"/>
       <c r="P21" s="7"/>
     </row>
     <row r="22" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="31">
+      <c r="B22" s="63"/>
+      <c r="C22" s="64">
         <v>44668</v>
       </c>
-      <c r="D22" s="65" t="s">
+      <c r="D22" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="67">
+      <c r="E22" s="23">
         <v>0.8</v>
       </c>
-      <c r="F22" s="68"/>
-      <c r="G22" s="32">
+      <c r="F22" s="24"/>
+      <c r="G22" s="61">
         <v>7</v>
       </c>
-      <c r="H22" s="27"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="58"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="58"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="29"/>
       <c r="P22" s="7"/>
     </row>
     <row r="23" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="60"/>
+      <c r="A23" s="63"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="31"/>
       <c r="P23" s="7"/>
     </row>
     <row r="24" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
       <c r="O24" s="11"/>
       <c r="P24" s="7"/>
     </row>
     <row r="25" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38" t="s">
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
       <c r="N25" s="19" t="s">
         <v>25</v>
       </c>
@@ -2413,215 +2443,215 @@
       <c r="P25" s="7"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="33"/>
+      <c r="B26" s="59"/>
       <c r="C26" s="20">
         <v>44669</v>
       </c>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
       <c r="N26" s="13"/>
       <c r="O26" s="11"/>
       <c r="P26" s="7"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="20">
         <v>44670</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
       <c r="N27" s="14"/>
       <c r="O27" s="15"/>
       <c r="P27" s="7"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="33"/>
+      <c r="B28" s="59"/>
       <c r="C28" s="20">
         <v>44671</v>
       </c>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
       <c r="N28" s="13"/>
       <c r="O28" s="11"/>
       <c r="P28" s="7"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="35"/>
+      <c r="B29" s="57"/>
       <c r="C29" s="20">
         <v>44672</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="58"/>
       <c r="N29" s="14"/>
       <c r="O29" s="15"/>
       <c r="P29" s="7"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="33"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="20">
         <v>44673</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
       <c r="N30" s="13"/>
       <c r="O30" s="11"/>
       <c r="P30" s="7"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="35"/>
+      <c r="B31" s="57"/>
       <c r="C31" s="20">
         <v>44674</v>
       </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
       <c r="N31" s="14"/>
       <c r="O31" s="15"/>
       <c r="P31" s="7"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="33"/>
+      <c r="B32" s="59"/>
       <c r="C32" s="20">
         <v>44675</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
       <c r="N32" s="13"/>
       <c r="O32" s="11"/>
       <c r="P32" s="7"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
-      <c r="O33" s="30"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="70"/>
+      <c r="N33" s="70"/>
+      <c r="O33" s="71"/>
       <c r="P33" s="7"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="23"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
+      <c r="L34" s="66"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="66"/>
+      <c r="O34" s="67"/>
       <c r="P34" s="7"/>
     </row>
     <row r="35" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="24"/>
-      <c r="O35" s="25"/>
+      <c r="A35" s="68"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="68"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="68"/>
+      <c r="O35" s="69"/>
       <c r="P35" s="7"/>
     </row>
     <row r="36" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2654,54 +2684,36 @@
     </row>
   </sheetData>
   <mergeCells count="94">
-    <mergeCell ref="H10:K11"/>
-    <mergeCell ref="E22:F23"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="E20:F21"/>
-    <mergeCell ref="L20:M21"/>
-    <mergeCell ref="L22:M23"/>
-    <mergeCell ref="N20:O21"/>
-    <mergeCell ref="N22:O23"/>
-    <mergeCell ref="H18:K19"/>
-    <mergeCell ref="L18:M19"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:O3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="H4:O4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="H5:O5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="H6:O6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="H7:O7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="G8:O8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:M31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:M32"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:M27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="D28:M28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:M29"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A34:O35"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="N12:O13"/>
+    <mergeCell ref="N14:O15"/>
+    <mergeCell ref="N16:O17"/>
+    <mergeCell ref="H16:K17"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="L16:M17"/>
+    <mergeCell ref="A33:O33"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="E10:F11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:F13"/>
+    <mergeCell ref="L14:M15"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="H12:K13"/>
+    <mergeCell ref="H14:K15"/>
     <mergeCell ref="N10:O11"/>
     <mergeCell ref="L12:M13"/>
     <mergeCell ref="A30:B30"/>
@@ -2718,36 +2730,54 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="A10:B11"/>
     <mergeCell ref="L10:M11"/>
-    <mergeCell ref="L14:M15"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="A12:B13"/>
-    <mergeCell ref="H12:K13"/>
-    <mergeCell ref="H14:K15"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="E10:F11"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:F13"/>
-    <mergeCell ref="A34:O35"/>
-    <mergeCell ref="A18:B19"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="A22:B23"/>
-    <mergeCell ref="N12:O13"/>
-    <mergeCell ref="N14:O15"/>
-    <mergeCell ref="N16:O17"/>
-    <mergeCell ref="H16:K17"/>
-    <mergeCell ref="A16:B17"/>
-    <mergeCell ref="L16:M17"/>
-    <mergeCell ref="A33:O33"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:M31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:M32"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:M27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:M28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:M29"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="G8:O8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:O5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="H6:O6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="H7:O7"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:O3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:O4"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="N20:O21"/>
+    <mergeCell ref="N22:O23"/>
+    <mergeCell ref="H18:K19"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="H10:K11"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="E20:F21"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.59027777777777779" bottom="0.39305555555555555" header="0.51111111111111107" footer="0.19652777777777777"/>
@@ -2757,11 +2787,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1EA73A2-7E29-4007-894A-D99E3477AC3F}">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2788,69 +2818,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="49"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="35"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="52"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="38"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
     <row r="3" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="53" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="55"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="41"/>
       <c r="P3" s="7"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
@@ -2859,514 +2889,514 @@
       <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="57"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="43"/>
       <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>1</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
       <c r="G5" s="8">
         <v>1</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="44"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="46"/>
       <c r="P5" s="7"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>2</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
       <c r="G6" s="9">
         <v>2</v>
       </c>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="47"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="49"/>
       <c r="P6" s="7"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>3</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
       <c r="G7" s="8">
         <v>3</v>
       </c>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="44"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="46"/>
       <c r="P7" s="7"/>
     </row>
     <row r="8" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="37" t="s">
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="40"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="52"/>
       <c r="P8" s="7"/>
     </row>
     <row r="9" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="63" t="s">
+      <c r="E9" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="64"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38" t="s">
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38" t="s">
+      <c r="M9" s="53"/>
+      <c r="N9" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="41"/>
+      <c r="O9" s="54"/>
       <c r="P9" s="7"/>
     </row>
     <row r="10" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="77">
+      <c r="B10" s="63"/>
+      <c r="C10" s="72">
         <v>44669</v>
       </c>
-      <c r="D10" s="65" t="s">
+      <c r="D10" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="76"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="32">
+      <c r="E10" s="78"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="61">
         <v>1</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="28"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="62"/>
       <c r="P10" s="7"/>
     </row>
     <row r="11" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="28"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="62"/>
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="77">
+      <c r="B12" s="63"/>
+      <c r="C12" s="72">
         <v>44670</v>
       </c>
-      <c r="D12" s="65" t="s">
+      <c r="D12" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="32">
+      <c r="E12" s="74"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="61">
         <v>2</v>
       </c>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="28"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="62"/>
       <c r="P12" s="7"/>
     </row>
     <row r="13" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="28"/>
+      <c r="A13" s="63"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="62"/>
       <c r="P13" s="7"/>
     </row>
     <row r="14" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="77">
+      <c r="B14" s="63"/>
+      <c r="C14" s="72">
         <v>44671</v>
       </c>
-      <c r="D14" s="65" t="s">
+      <c r="D14" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="72"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="32">
+      <c r="E14" s="74"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="61">
         <v>3</v>
       </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="28"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="62"/>
       <c r="P14" s="7"/>
     </row>
     <row r="15" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="28"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="62"/>
       <c r="P15" s="7"/>
     </row>
     <row r="16" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="77">
+      <c r="B16" s="63"/>
+      <c r="C16" s="72">
         <v>44672</v>
       </c>
-      <c r="D16" s="65" t="s">
+      <c r="D16" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="72"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="32">
+      <c r="E16" s="74"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="61">
         <v>4</v>
       </c>
-      <c r="H16" s="27" t="s">
+      <c r="H16" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27" t="s">
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27" t="s">
+      <c r="M16" s="22"/>
+      <c r="N16" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="O16" s="28"/>
+      <c r="O16" s="62"/>
       <c r="P16" s="7"/>
     </row>
     <row r="17" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="28"/>
+      <c r="A17" s="63"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="62"/>
       <c r="P17" s="7"/>
     </row>
     <row r="18" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="77">
+      <c r="B18" s="63"/>
+      <c r="C18" s="72">
         <v>44673</v>
       </c>
-      <c r="D18" s="65" t="s">
+      <c r="D18" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="32">
+      <c r="E18" s="74"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="61">
         <v>5</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="H18" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27" t="s">
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27" t="s">
+      <c r="M18" s="22"/>
+      <c r="N18" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="O18" s="28"/>
+      <c r="O18" s="62"/>
       <c r="P18" s="7"/>
     </row>
     <row r="19" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="28"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="62"/>
       <c r="P19" s="7"/>
     </row>
     <row r="20" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="77">
+      <c r="B20" s="63"/>
+      <c r="C20" s="72">
         <v>44674</v>
       </c>
-      <c r="D20" s="65" t="s">
+      <c r="D20" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="72"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="32">
+      <c r="E20" s="74"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="61">
         <v>6</v>
       </c>
-      <c r="H20" s="27"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="58"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="58"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="29"/>
       <c r="P20" s="7"/>
     </row>
     <row r="21" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="60"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="31"/>
       <c r="P21" s="7"/>
     </row>
     <row r="22" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="26"/>
-      <c r="C22" s="77">
+      <c r="B22" s="63"/>
+      <c r="C22" s="72">
         <v>44675</v>
       </c>
-      <c r="D22" s="65" t="s">
+      <c r="D22" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="72"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="32">
+      <c r="E22" s="74"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="61">
         <v>7</v>
       </c>
-      <c r="H22" s="27"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="58"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="58"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="58"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="29"/>
       <c r="P22" s="7"/>
     </row>
     <row r="23" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="60"/>
+      <c r="A23" s="63"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="31"/>
       <c r="P23" s="7"/>
     </row>
     <row r="24" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
       <c r="O24" s="11"/>
       <c r="P24" s="7"/>
     </row>
     <row r="25" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38" t="s">
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="38"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
       <c r="N25" s="19" t="s">
         <v>25</v>
       </c>
@@ -3374,223 +3404,223 @@
       <c r="P25" s="7"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="78">
+      <c r="B26" s="59"/>
+      <c r="C26" s="21">
         <v>44676</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
       <c r="N26" s="13"/>
       <c r="O26" s="11"/>
       <c r="P26" s="7"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="78">
+      <c r="B27" s="57"/>
+      <c r="C27" s="21">
         <v>44677</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
       <c r="N27" s="14"/>
       <c r="O27" s="15"/>
       <c r="P27" s="7"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="78">
+      <c r="B28" s="59"/>
+      <c r="C28" s="21">
         <v>44678</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
       <c r="N28" s="13"/>
       <c r="O28" s="11"/>
       <c r="P28" s="7"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="78">
+      <c r="B29" s="57"/>
+      <c r="C29" s="21">
         <v>44679</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="36"/>
-      <c r="L29" s="36"/>
-      <c r="M29" s="36"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="58"/>
       <c r="N29" s="14"/>
       <c r="O29" s="15"/>
       <c r="P29" s="7"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="78">
+      <c r="B30" s="59"/>
+      <c r="C30" s="21">
         <v>44680</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
       <c r="N30" s="13"/>
       <c r="O30" s="11"/>
       <c r="P30" s="7"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="78">
+      <c r="B31" s="57"/>
+      <c r="C31" s="21">
         <v>44681</v>
       </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
       <c r="N31" s="14"/>
       <c r="O31" s="15"/>
       <c r="P31" s="7"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="C32" s="78">
+      <c r="B32" s="59"/>
+      <c r="C32" s="21">
         <v>44682</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
       <c r="N32" s="13"/>
       <c r="O32" s="11"/>
       <c r="P32" s="7"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
-      <c r="O33" s="30"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="70"/>
+      <c r="N33" s="70"/>
+      <c r="O33" s="71"/>
       <c r="P33" s="7"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="23"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
+      <c r="L34" s="66"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="66"/>
+      <c r="O34" s="67"/>
       <c r="P34" s="7"/>
     </row>
     <row r="35" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="24"/>
-      <c r="N35" s="24"/>
-      <c r="O35" s="25"/>
+      <c r="A35" s="68"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="68"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="68"/>
+      <c r="O35" s="69"/>
       <c r="P35" s="7"/>
     </row>
     <row r="36" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3623,6 +3653,7 @@
     </row>
   </sheetData>
   <mergeCells count="94">
+    <mergeCell ref="A33:O33"/>
     <mergeCell ref="A34:O35"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="D30:M30"/>
@@ -3630,17 +3661,17 @@
     <mergeCell ref="D31:M31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="D32:M32"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:M27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="D28:M28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="D29:M29"/>
-    <mergeCell ref="A33:O33"/>
+    <mergeCell ref="L22:M23"/>
     <mergeCell ref="N22:O23"/>
     <mergeCell ref="A24:N24"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="D25:M25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="D27:M27"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="D26:M26"/>
     <mergeCell ref="A22:B23"/>
@@ -3649,7 +3680,6 @@
     <mergeCell ref="E22:F23"/>
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="H22:K23"/>
-    <mergeCell ref="L22:M23"/>
     <mergeCell ref="L18:M19"/>
     <mergeCell ref="N18:O19"/>
     <mergeCell ref="A20:B21"/>
@@ -3718,9 +3748,969 @@
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:O4"/>
   </mergeCells>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.59027777777777779" bottom="0.39305555555555555" header="0.51111111111111107" footer="0.19652777777777777"/>
+  <pageSetup paperSize="9" scale="95" firstPageNumber="4294963191" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:R40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.19921875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="3.59765625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8" style="3" customWidth="1"/>
+    <col min="4" max="4" width="36" style="3" customWidth="1"/>
+    <col min="5" max="5" width="4.19921875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="5.59765625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="4.8984375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="6.09765625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.09765625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="6.59765625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="4.5" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.09765625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="7.19921875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.8984375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="8.59765625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="6.8984375" style="3" customWidth="1"/>
+    <col min="17" max="17" width="9" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.69921875" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+    </row>
+    <row r="3" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+    </row>
+    <row r="4" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="9">
+        <v>2</v>
+      </c>
+      <c r="H6" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>3</v>
+      </c>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="8">
+        <v>3</v>
+      </c>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="45"/>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="56"/>
+      <c r="G9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" s="54"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="63"/>
+      <c r="C10" s="72">
+        <v>44676</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="78"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="61">
+        <v>1</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="62"/>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="63"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="62"/>
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="72">
+        <v>44677</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="74"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="61">
+        <v>2</v>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="62"/>
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="63"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="63"/>
+      <c r="C14" s="72">
+        <v>44678</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="74"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="61">
+        <v>3</v>
+      </c>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="7"/>
+    </row>
+    <row r="16" spans="1:18" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="63"/>
+      <c r="C16" s="72">
+        <v>44679</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="74"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="61">
+        <v>4</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="62"/>
+      <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="63"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="62"/>
+      <c r="P17" s="7"/>
+    </row>
+    <row r="18" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="63"/>
+      <c r="C18" s="72">
+        <v>44680</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="61">
+        <v>5</v>
+      </c>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="62"/>
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="63"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="63" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="63"/>
+      <c r="C20" s="72">
+        <v>44681</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="61">
+        <v>6</v>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="7"/>
+    </row>
+    <row r="21" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="63"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="7"/>
+    </row>
+    <row r="22" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="63"/>
+      <c r="C22" s="72">
+        <v>44682</v>
+      </c>
+      <c r="D22" s="27"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="61">
+        <v>7</v>
+      </c>
+      <c r="H22" s="22"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="7"/>
+    </row>
+    <row r="23" spans="1:16" ht="12.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="63"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="76"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="7"/>
+    </row>
+    <row r="24" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="7"/>
+    </row>
+    <row r="25" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
+      <c r="M25" s="53"/>
+      <c r="N25" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="O25" s="12"/>
+      <c r="P25" s="7"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="59"/>
+      <c r="C26" s="21">
+        <v>44683</v>
+      </c>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="7"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="57"/>
+      <c r="C27" s="21">
+        <v>44684</v>
+      </c>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="7"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="59"/>
+      <c r="C28" s="21">
+        <v>44685</v>
+      </c>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="7"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="57"/>
+      <c r="C29" s="21">
+        <v>44686</v>
+      </c>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="58"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="7"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="59"/>
+      <c r="C30" s="21">
+        <v>44687</v>
+      </c>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="7"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A31" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="57"/>
+      <c r="C31" s="21">
+        <v>44688</v>
+      </c>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="7"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A32" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="59"/>
+      <c r="C32" s="21">
+        <v>44689</v>
+      </c>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="7"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="70"/>
+      <c r="N33" s="70"/>
+      <c r="O33" s="71"/>
+      <c r="P33" s="7"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
+      <c r="L34" s="66"/>
+      <c r="M34" s="66"/>
+      <c r="N34" s="66"/>
+      <c r="O34" s="67"/>
+      <c r="P34" s="7"/>
+    </row>
+    <row r="35" spans="1:16" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="68"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="68"/>
+      <c r="J35" s="68"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="68"/>
+      <c r="N35" s="68"/>
+      <c r="O35" s="69"/>
+      <c r="P35" s="7"/>
+    </row>
+    <row r="36" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C39" s="7"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D40" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="94">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:O3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:O4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:O5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="H6:O6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="H7:O7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="G8:O8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="L10:M11"/>
+    <mergeCell ref="N10:O11"/>
+    <mergeCell ref="A12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:K13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="N12:O13"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:K11"/>
+    <mergeCell ref="L14:M15"/>
+    <mergeCell ref="N14:O15"/>
+    <mergeCell ref="A16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:K17"/>
+    <mergeCell ref="L16:M17"/>
+    <mergeCell ref="N16:O17"/>
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:K15"/>
+    <mergeCell ref="L18:M19"/>
+    <mergeCell ref="N18:O19"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:K21"/>
+    <mergeCell ref="L20:M21"/>
+    <mergeCell ref="N20:O21"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:K19"/>
+    <mergeCell ref="N22:O23"/>
+    <mergeCell ref="A24:N24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:M25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="D27:M27"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="D26:M26"/>
+    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:K23"/>
+    <mergeCell ref="L22:M23"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="D28:M28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:M29"/>
+    <mergeCell ref="A33:O33"/>
+    <mergeCell ref="A34:O35"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:M30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:M31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:M32"/>
+  </mergeCells>
   <phoneticPr fontId="38" type="noConversion"/>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.59027777777777779" bottom="0.39305555555555555" header="0.51111111111111107" footer="0.19652777777777777"/>
   <pageSetup paperSize="9" scale="95" firstPageNumber="4294963191" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5037E1DB-AAE1-44E4-A965-10D5E1C18A6A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>